<commit_message>
update Cong tac an toan
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/DK/DanhSachTaiNan-download.xlsx
+++ b/QUANGHANH2/excel/DK/DanhSachTaiNan-download.xlsx
@@ -2,9 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7785"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Mã nhân viên</t>
   </si>
@@ -60,7 +65,25 @@
     <t>CA 1</t>
   </si>
   <si>
-    <t>23/10/2019</t>
+    <t>17/11/2019</t>
+  </si>
+  <si>
+    <t>8022</t>
+  </si>
+  <si>
+    <t>Cơ điện vận tải</t>
+  </si>
+  <si>
+    <t>dsgfsg</t>
+  </si>
+  <si>
+    <t>25/10/2019</t>
+  </si>
+  <si>
+    <t>fgdh</t>
+  </si>
+  <si>
+    <t>15/10/2019</t>
   </si>
 </sst>
 </file>
@@ -72,18 +95,18 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -125,18 +148,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -414,74 +436,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="15.5" customWidth="1" style="3"/>
-    <col min="2" max="2" bestFit="1" width="15.8984375" customWidth="1" style="3"/>
-    <col min="3" max="3" bestFit="1" width="7.8984375" customWidth="1" style="3"/>
-    <col min="4" max="4" width="18.8984375" customWidth="1" style="3"/>
-    <col min="5" max="5" width="14" customWidth="1" style="3"/>
-    <col min="6" max="6" bestFit="1" width="4.296875" customWidth="1" style="3"/>
-    <col min="7" max="7" width="15.69921875" customWidth="1" style="3"/>
-    <col min="8" max="16384" width="8.796875" customWidth="1" style="3"/>
+    <col min="1" max="1" bestFit="1" width="15.46484375" customWidth="1" style="2"/>
+    <col min="2" max="2" bestFit="1" width="15.86328125" customWidth="1" style="2"/>
+    <col min="3" max="3" bestFit="1" width="7.86328125" customWidth="1" style="2"/>
+    <col min="4" max="4" width="18.86328125" customWidth="1" style="2"/>
+    <col min="5" max="5" width="14" customWidth="1" style="2"/>
+    <col min="6" max="6" bestFit="1" width="4.265625" customWidth="1" style="2"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1" style="2"/>
+    <col min="8" max="16384" width="8.796875" customWidth="1" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.4" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="17.25" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>